<commit_message>
10 uF cap FR
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/calibration20160913.xlsx
+++ b/myESC-Particle-DEV/saves/calibration20160913.xlsx
@@ -2243,6 +2243,488 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Cal!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calc PCNF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:forward val="200"/>
+            <c:backward val="9"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.26646434820647419"/>
+                  <c:y val="1.8101851851851852E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Cal!$F$2:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>18.954000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.065999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.970400000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.176200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.176200000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.774099999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.774099999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>68.166200000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>77.8596</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88.417000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100.6914</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>126.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>155.69400000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Cal!$M$2:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6.1305687199999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.093358079999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.026802</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.594195554999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.493464079999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.429051919999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.114734079999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.444933119999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.824043579999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.627237499999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.852740479999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.272622720000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.910257919999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26.324791579999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.97638208</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.97638208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="485872592"/>
+        <c:axId val="485871808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="485872592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ESC Power, W</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485871808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="485871808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485872592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr/>
@@ -2503,7 +2985,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3136,6 +4174,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3471,7 +4539,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" activeCellId="4" sqref="B1:B1048576 D1:D1048576 E1:E1048576 F1:F1048576 K1:K1048576"/>
+      <selection activeCell="M1" activeCellId="1" sqref="F1:F1048576 M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
debug closed loop cleanup
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/calibration20160913.xlsx
+++ b/myESC-Particle-DEV/saves/calibration20160913.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>throttleFlt, deg</t>
   </si>
@@ -222,6 +222,9 @@
   <si>
     <t>P_LT_NG</t>
   </si>
+  <si>
+    <t>Calc Throttle from Ng, deg</t>
+  </si>
 </sst>
 </file>
 
@@ -285,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,6 +342,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,8 +891,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206457248"/>
-        <c:axId val="206459992"/>
+        <c:axId val="474309080"/>
+        <c:axId val="474310648"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1177,11 +1183,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206460384"/>
-        <c:axId val="206457640"/>
+        <c:axId val="474308688"/>
+        <c:axId val="474304376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="206457248"/>
+        <c:axId val="474309080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="115"/>
@@ -1303,12 +1309,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206459992"/>
+        <c:crossAx val="474310648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206459992"/>
+        <c:axId val="474310648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1365,12 +1371,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206457248"/>
+        <c:crossAx val="474309080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206457640"/>
+        <c:axId val="474304376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20000"/>
@@ -1414,12 +1420,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206460384"/>
+        <c:crossAx val="474308688"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206460384"/>
+        <c:axId val="474308688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1429,7 +1435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206457640"/>
+        <c:crossAx val="474304376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1766,8 +1772,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206461168"/>
-        <c:axId val="206461952"/>
+        <c:axId val="474306728"/>
+        <c:axId val="474307120"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1930,11 +1936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206458032"/>
-        <c:axId val="206456856"/>
+        <c:axId val="473523040"/>
+        <c:axId val="474307512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="206461168"/>
+        <c:axId val="474306728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="216"/>
@@ -2034,12 +2040,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206461952"/>
+        <c:crossAx val="474307120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206461952"/>
+        <c:axId val="474307120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2153,13 +2159,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206461168"/>
+        <c:crossAx val="474306728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206456856"/>
+        <c:axId val="474307512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -2204,13 +2210,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206458032"/>
+        <c:crossAx val="473523040"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206458032"/>
+        <c:axId val="473523040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2220,7 +2226,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206456856"/>
+        <c:crossAx val="474307512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2580,11 +2586,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="204917064"/>
-        <c:axId val="208531976"/>
+        <c:axId val="473517944"/>
+        <c:axId val="473519512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="204917064"/>
+        <c:axId val="473517944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="115"/>
@@ -2699,12 +2705,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208531976"/>
+        <c:crossAx val="473519512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="208531976"/>
+        <c:axId val="473519512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20945"/>
@@ -2824,7 +2830,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204917064"/>
+        <c:crossAx val="473517944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3162,11 +3168,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208532368"/>
-        <c:axId val="208538248"/>
+        <c:axId val="473520296"/>
+        <c:axId val="473522256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="208532368"/>
+        <c:axId val="473520296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -3285,12 +3291,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208538248"/>
+        <c:crossAx val="473522256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="208538248"/>
+        <c:axId val="473522256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16194"/>
@@ -3410,7 +3416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208532368"/>
+        <c:crossAx val="473520296"/>
         <c:crossesAt val="-1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3489,7 +3495,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3596,11 +3601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208532760"/>
-        <c:axId val="208533152"/>
+        <c:axId val="473521080"/>
+        <c:axId val="472310216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="208532760"/>
+        <c:axId val="473521080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20945"/>
@@ -3630,19 +3635,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208533152"/>
+        <c:crossAx val="472310216"/>
         <c:crossesAt val="-5000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="208533152"/>
+        <c:axId val="472310216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16194"/>
@@ -3667,14 +3671,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208532760"/>
+        <c:crossAx val="473521080"/>
         <c:crossesAt val="-5000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3824,7 +3827,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3919,11 +3921,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208534328"/>
-        <c:axId val="208533544"/>
+        <c:axId val="472315312"/>
+        <c:axId val="472314136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="208534328"/>
+        <c:axId val="472315312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16194"/>
@@ -3976,7 +3978,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4043,12 +4044,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208533544"/>
+        <c:crossAx val="472314136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="208533544"/>
+        <c:axId val="472314136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20000"/>
@@ -4095,7 +4096,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4162,7 +4162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="208534328"/>
+        <c:crossAx val="472315312"/>
         <c:crossesAt val="-5000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7091,7 +7091,7 @@
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>472440</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -7470,10 +7470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC20"/>
+  <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7492,20 +7492,20 @@
     <col min="14" max="14" width="4.21875" style="1" customWidth="1"/>
     <col min="15" max="16" width="7.6640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="6.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="6.109375" customWidth="1"/>
-    <col min="21" max="21" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" customWidth="1"/>
-    <col min="24" max="24" width="11.5546875" customWidth="1"/>
-    <col min="25" max="25" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.88671875" customWidth="1"/>
-    <col min="27" max="27" width="10" customWidth="1"/>
-    <col min="28" max="28" width="7.5546875" customWidth="1"/>
-    <col min="29" max="29" width="7.88671875" customWidth="1"/>
+    <col min="18" max="19" width="7.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" customWidth="1"/>
+    <col min="22" max="22" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" customWidth="1"/>
+    <col min="25" max="25" width="11.5546875" customWidth="1"/>
+    <col min="26" max="26" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.88671875" customWidth="1"/>
+    <col min="28" max="28" width="10" customWidth="1"/>
+    <col min="29" max="29" width="7.5546875" customWidth="1"/>
+    <col min="30" max="30" width="7.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -7561,34 +7561,37 @@
         <v>30</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="6">
+      <c r="V1" s="6">
         <v>2</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="Y1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Z1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="AA1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AB1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AC1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AD1" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1.1399999999999999</v>
       </c>
@@ -7631,11 +7634,11 @@
         <v>116.07661056297157</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" ref="M2:M17" si="1">L2*60/$U$1</f>
+        <f t="shared" ref="M2:M17" si="1">L2*60/$V$1</f>
         <v>3482.2983168891469</v>
       </c>
       <c r="N2" s="3">
-        <f t="shared" ref="N2:N15" si="2">M2/$U$4*100</f>
+        <f t="shared" ref="N2:N15" si="2">M2/$V$4*100</f>
         <v>16.625556200425613</v>
       </c>
       <c r="O2" s="3">
@@ -7647,49 +7650,53 @@
         <v>61</v>
       </c>
       <c r="Q2" s="3">
-        <f t="shared" ref="Q2:Q14" si="3">O2/$U$4*100</f>
+        <f t="shared" ref="Q2:Q14" si="3">O2/$V$4*100</f>
         <v>38.638747148677588</v>
       </c>
       <c r="R2" s="3">
-        <f>$U$10*LN(B2)+$U$11</f>
+        <f>$V$10*LN(B2)+$V$11</f>
         <v>8196.636802490626</v>
       </c>
-      <c r="S2" s="3">
-        <f>C2*C2*$U$7+C2*$U$8+$U$9</f>
+      <c r="S2" s="23">
+        <f>EXP((R2-$V$11)/$V$10)</f>
+        <v>61.000000000000007</v>
+      </c>
+      <c r="T2" s="3">
+        <f>C2*C2*$V$7+C2*$V$8+$V$9</f>
         <v>4005.3848106256592</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="6">
+      <c r="V2" s="6">
         <v>4800</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="X2" s="11">
+      <c r="Y2" s="11">
         <v>0</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>0</v>
       </c>
-      <c r="Z2">
-        <f>Y2*$U$4/100</f>
+      <c r="AA2">
+        <f>Z2*$V$4/100</f>
         <v>0</v>
       </c>
-      <c r="AA2">
-        <f>EXP((Z2-$U$11)/$U$10)</f>
+      <c r="AB2">
+        <f>EXP((AA2-$V$11)/$V$10)</f>
         <v>40.65722380177391</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>-5000</v>
       </c>
-      <c r="AC2">
-        <f>AB2/$U$4*100</f>
+      <c r="AD2">
+        <f>AC2/$V$4*100</f>
         <v>-23.871527777777779</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="10">
         <v>65</v>
@@ -7750,46 +7757,50 @@
         <v>44.828158923956003</v>
       </c>
       <c r="R3" s="3">
-        <f t="shared" ref="R3:R14" si="9">$U$10*LN(B3)+$U$11</f>
+        <f t="shared" ref="R3:R14" si="9">$V$10*LN(B3)+$V$11</f>
         <v>9479.8503504825057</v>
       </c>
-      <c r="S3" s="3">
-        <f t="shared" ref="S3:S17" si="10">C3*C3*$U$7+C3*$U$8+$U$9</f>
+      <c r="S3" s="23">
+        <f t="shared" ref="S3:S14" si="10">EXP((R3-$V$11)/$V$10)</f>
+        <v>64.999999999999986</v>
+      </c>
+      <c r="T3" s="3">
+        <f t="shared" ref="T3:T17" si="11">C3*C3*$V$7+C3*$V$8+$V$9</f>
         <v>4987.9393693866259</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="6">
+      <c r="V3" s="6">
         <v>12</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="X3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="X3" s="11">
+      <c r="Y3" s="11">
         <v>3.3</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>100</v>
       </c>
-      <c r="Z3">
-        <f>Y3*$U$4/100</f>
+      <c r="AA3">
+        <f>Z3*$V$4/100</f>
         <v>20945.454545454544</v>
       </c>
-      <c r="AA3">
-        <f>EXP((Z3-$U$11)/$U$10)</f>
+      <c r="AB3">
+        <f>EXP((AA3-$V$11)/$V$10)</f>
         <v>114.65000595374373</v>
       </c>
-      <c r="AB3">
-        <f>Z3*Coupling!$C$8+Coupling!$C$9</f>
+      <c r="AC3">
+        <f>AA3*Coupling!$C$8+Coupling!$C$9</f>
         <v>16194.279022996247</v>
       </c>
-      <c r="AC3">
-        <f>AB3/$U$4*100</f>
+      <c r="AD3">
+        <f>AC3/$V$4*100</f>
         <v>77.316436307707775</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="10">
         <v>70</v>
@@ -7853,42 +7864,46 @@
         <f t="shared" si="9"/>
         <v>10977.114633516147</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="23">
         <f t="shared" si="10"/>
+        <v>70.000000000000028</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" si="11"/>
         <v>6485.4664870301367</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="13">
-        <f>U2*U3/V4</f>
+      <c r="V4" s="13">
+        <f>V2*V3/W4</f>
         <v>20945.454545454544</v>
       </c>
-      <c r="V4" s="6">
+      <c r="W4" s="6">
         <v>2.75</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>31</v>
       </c>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="14">
-        <f>INDEX(LINEST(Y$2:Y$3,$X$2:$X$3),1)</f>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="14">
+        <f>INDEX(LINEST(Z$2:Z$3,$Y$2:$Y$3),1)</f>
         <v>30.303030303030305</v>
       </c>
-      <c r="Z4" s="14">
-        <f>INDEX(LINEST($Z$2:$Z$3,$X$2:$X$3),1)</f>
+      <c r="AA4" s="14">
+        <f>INDEX(LINEST($AA$2:$AA$3,$Y$2:$Y$3),1)</f>
         <v>6347.1074380165273</v>
       </c>
-      <c r="AB4" s="14">
-        <f t="shared" ref="AB4:AC4" si="11">INDEX(LINEST(AB$2:AB$3,$X$2:$X$3),1)</f>
+      <c r="AC4" s="14">
+        <f t="shared" ref="AC4:AD4" si="12">INDEX(LINEST(AC$2:AC$3,$Y$2:$Y$3),1)</f>
         <v>6422.5087948473483</v>
       </c>
-      <c r="AC4" s="14">
-        <f t="shared" si="11"/>
+      <c r="AD4" s="14">
+        <f t="shared" si="12"/>
         <v>30.663019419844112</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="10">
         <v>75</v>
@@ -7952,36 +7967,40 @@
         <f t="shared" si="9"/>
         <v>12371.034332830881</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="23">
         <f t="shared" si="10"/>
+        <v>74.999999999999972</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" si="11"/>
         <v>7829.7506403399002</v>
       </c>
-      <c r="V5" s="22">
+      <c r="W5" s="22">
         <f>Coupling!J5</f>
         <v>216</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>13</v>
       </c>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="14">
-        <f>INDEX(LINEST(Y$2:Y$3,$X$2:$X$3),2)</f>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="14">
+        <f>INDEX(LINEST(Z$2:Z$3,$Y$2:$Y$3),2)</f>
         <v>0</v>
       </c>
-      <c r="Z5" s="14">
-        <f>INDEX(LINEST($Z$2:$Z$3,$X$2:$X$3),2)</f>
+      <c r="AA5" s="14">
+        <f>INDEX(LINEST($AA$2:$AA$3,$Y$2:$Y$3),2)</f>
         <v>1.8189894035458565E-12</v>
       </c>
-      <c r="AB5" s="14">
-        <f t="shared" ref="AB5:AC5" si="12">INDEX(LINEST(AB$2:AB$3,$X$2:$X$3),2)</f>
+      <c r="AC5" s="14">
+        <f t="shared" ref="AC5:AD5" si="13">INDEX(LINEST(AC$2:AC$3,$Y$2:$Y$3),2)</f>
         <v>-5000.0000000000009</v>
       </c>
-      <c r="AC5" s="14">
-        <f t="shared" si="12"/>
+      <c r="AD5" s="14">
+        <f t="shared" si="13"/>
         <v>-23.871527777777782</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="10">
         <v>77</v>
@@ -8045,24 +8064,28 @@
         <f t="shared" si="9"/>
         <v>12902.744547319715</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="23">
         <f t="shared" si="10"/>
+        <v>77.000000000000014</v>
+      </c>
+      <c r="T6" s="3">
+        <f t="shared" si="11"/>
         <v>8309.2357673476217</v>
       </c>
-      <c r="Y6" s="14" t="s">
+      <c r="Z6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="Z6" s="14" t="s">
+      <c r="AA6" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="AB6" s="14" t="s">
+      <c r="AC6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AD6" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="10">
         <v>79</v>
@@ -8126,26 +8149,30 @@
         <f t="shared" si="9"/>
         <v>13420.819652760169</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="23">
         <f t="shared" si="10"/>
+        <v>79</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" si="11"/>
         <v>8813.4082722245112</v>
       </c>
-      <c r="T7" s="5" t="s">
+      <c r="U7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="U7" s="13">
+      <c r="V7" s="13">
         <f>INDEX(LINEST($M$2:$M$17,$C$2:$C$17^{1,2},FALSE,FALSE),1)</f>
         <v>-586.95945682909951</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>39</v>
       </c>
-      <c r="Y7" s="20"/>
       <c r="Z7" s="20"/>
-      <c r="AB7" s="20"/>
+      <c r="AA7" s="20"/>
       <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
     </row>
-    <row r="8" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="10">
         <v>81</v>
@@ -8209,20 +8236,24 @@
         <f t="shared" si="9"/>
         <v>13925.941513925834</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="23">
         <f t="shared" si="10"/>
+        <v>81.000000000000028</v>
+      </c>
+      <c r="T8" s="3">
+        <f t="shared" si="11"/>
         <v>9186.6071914448148</v>
       </c>
-      <c r="T8" s="5"/>
-      <c r="U8" s="14">
+      <c r="U8" s="5"/>
+      <c r="V8" s="14">
         <f>INDEX(LINEST($M$2:$M$17,$C$2:$C$17^{1,2},FALSE,FALSE),2)</f>
         <v>7734.3373856241196</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>1.55</v>
       </c>
@@ -8288,20 +8319,24 @@
         <f t="shared" si="9"/>
         <v>14540.08673420093</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="23">
         <f t="shared" si="10"/>
+        <v>83.500000000000014</v>
+      </c>
+      <c r="T9" s="3">
+        <f t="shared" si="11"/>
         <v>9920.3267056179102</v>
       </c>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5">
+      <c r="U9" s="5"/>
+      <c r="V9" s="5">
         <f>INDEX(LINEST($M$2:$M$17,$C$2:$C$17^{1,2},FALSE,FALSE),3)</f>
         <v>0</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="10">
         <v>88</v>
@@ -8365,19 +8400,23 @@
         <f t="shared" si="9"/>
         <v>15600.589044072636</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10" s="23">
         <f t="shared" si="10"/>
+        <v>88.000000000000028</v>
+      </c>
+      <c r="T10" s="3">
+        <f t="shared" si="11"/>
         <v>10696.113330291821</v>
       </c>
-      <c r="T10" s="5" t="s">
+      <c r="U10" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="U10" s="5">
+      <c r="V10" s="5">
         <f>INDEX(LINEST($O$2:$O$14,$K$2:$K$14),1)</f>
         <v>20203.822065564778</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="10">
         <v>92</v>
@@ -8441,17 +8480,21 @@
         <f t="shared" si="9"/>
         <v>16498.684545554497</v>
       </c>
-      <c r="S11" s="3">
+      <c r="S11" s="23">
         <f t="shared" si="10"/>
+        <v>92.000000000000014</v>
+      </c>
+      <c r="T11" s="3">
+        <f t="shared" si="11"/>
         <v>11737.527088303092</v>
       </c>
-      <c r="T11" s="5"/>
-      <c r="U11" s="14">
+      <c r="U11" s="5"/>
+      <c r="V11" s="14">
         <f>INDEX(LINEST($O$2:$O$14,$K$2:$K$14),2)</f>
         <v>-74858.727283247674</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>1.79</v>
       </c>
@@ -8517,24 +8560,28 @@
         <f t="shared" si="9"/>
         <v>17146.991143136882</v>
       </c>
-      <c r="S12" s="3">
+      <c r="S12" s="23">
         <f t="shared" si="10"/>
+        <v>95</v>
+      </c>
+      <c r="T12" s="3">
+        <f t="shared" si="11"/>
         <v>12466.004780756575</v>
       </c>
-      <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
-      <c r="X12" s="18" t="s">
+      <c r="W12" s="7"/>
+      <c r="Y12" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="Y12" s="18" t="s">
+      <c r="Z12" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="10">
         <v>100</v>
@@ -8598,28 +8645,32 @@
         <f t="shared" si="9"/>
         <v>18183.311736099597</v>
       </c>
-      <c r="S13" s="3">
+      <c r="S13" s="23">
         <f t="shared" si="10"/>
+        <v>100.00000000000004</v>
+      </c>
+      <c r="T13" s="3">
+        <f t="shared" si="11"/>
         <v>13335.357791133223</v>
       </c>
-      <c r="V13" s="7"/>
-      <c r="W13" s="5" t="s">
+      <c r="W13" s="7"/>
+      <c r="X13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="X13" s="5">
+      <c r="Y13" s="5">
         <v>0</v>
       </c>
-      <c r="Y13" s="5">
+      <c r="Z13" s="5">
         <v>40</v>
       </c>
-      <c r="Z13" s="5" t="s">
+      <c r="AA13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="10">
         <v>105</v>
@@ -8683,28 +8734,32 @@
         <f t="shared" si="9"/>
         <v>19169.059531528474</v>
       </c>
-      <c r="S14" s="3">
+      <c r="S14" s="23">
         <f t="shared" si="10"/>
+        <v>104.99999999999997</v>
+      </c>
+      <c r="T14" s="3">
+        <f t="shared" si="11"/>
         <v>14379.787973212338</v>
       </c>
-      <c r="V14" s="7"/>
-      <c r="W14" s="5" t="s">
+      <c r="W14" s="7"/>
+      <c r="X14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="X14" s="5">
+      <c r="Y14" s="5">
         <v>5</v>
       </c>
-      <c r="Y14" s="5">
+      <c r="Z14" s="5">
         <v>115</v>
       </c>
-      <c r="Z14" s="5" t="s">
+      <c r="AA14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="10">
         <v>110</v>
@@ -8739,26 +8794,27 @@
         <v>73.113408201463344</v>
       </c>
       <c r="Q15" s="3">
-        <f>O18/$U$4*100</f>
+        <f>O18/$V$4*100</f>
         <v>0</v>
       </c>
       <c r="R15" s="3"/>
-      <c r="S15" s="3">
-        <f t="shared" si="10"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3">
+        <f t="shared" si="11"/>
         <v>15328.502950436463</v>
       </c>
-      <c r="T15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="Y15" s="7">
-        <f>(Y14-Y13)/(X14-X13)</f>
+      <c r="U15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="Z15" s="7">
+        <f>(Z14-Z13)/(Y14-Y13)</f>
         <v>15</v>
       </c>
-      <c r="AA15" s="5">
-        <f>(AA14-AA13)/(X14-X13)</f>
+      <c r="AB15" s="5">
+        <f>(AB14-AB13)/(Y14-Y13)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>2.14</v>
       </c>
@@ -8793,22 +8849,23 @@
       <c r="N16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3">
-        <f>C16*C16*$U$7+C16*$U$8+$U$9</f>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3">
+        <f>C16*C16*$V$7+C16*$V$8+$V$9</f>
         <v>16512.246590743318</v>
       </c>
-      <c r="T16" s="7"/>
       <c r="U16" s="7"/>
-      <c r="Y16" s="7">
-        <f>Y14-Y15*X14</f>
+      <c r="V16" s="7"/>
+      <c r="Z16" s="7">
+        <f>Z14-Z15*Y14</f>
         <v>40</v>
       </c>
-      <c r="AA16" s="5">
-        <f>AA14-AA15*(X14-X13)</f>
+      <c r="AB16" s="5">
+        <f>AB14-AB15*(Y14-Y13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="10">
         <v>120</v>
@@ -8841,21 +8898,23 @@
       <c r="N17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="3">
-        <f t="shared" si="10"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3">
+        <f t="shared" si="11"/>
         <v>16512.246590743318</v>
       </c>
-      <c r="Y17" s="7" t="s">
+      <c r="Z17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AA17" s="5" t="s">
+      <c r="AB17" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="N20" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>